<commit_message>
update methods in CW
</commit_message>
<xml_diff>
--- a/Tables/ODM2_DarwinCore_StreamHabitat_ExchangeSpecifications.xlsx
+++ b/Tables/ODM2_DarwinCore_StreamHabitat_ExchangeSpecifications.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="505" uniqueCount="505">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="512" uniqueCount="512">
   <si>
     <t xml:space="preserve">TermID</t>
   </si>
@@ -1344,6 +1344,9 @@
     <t xml:space="preserve">REACH_LENGTH</t>
   </si>
   <si>
+    <t xml:space="preserve">www.monitoringresources.org/Document/Method/Details/3807</t>
+  </si>
+  <si>
     <t xml:space="preserve">TOT_RCH_LEN</t>
   </si>
   <si>
@@ -1392,15 +1395,27 @@
     <t xml:space="preserve">ave_residual_depth</t>
   </si>
   <si>
+    <t xml:space="preserve">www.monitoringresources.org/Document/Method/Details/6844</t>
+  </si>
+  <si>
     <t xml:space="preserve">RES_PL_DEP</t>
   </si>
   <si>
     <t xml:space="preserve">ResPoolDepthAvg</t>
   </si>
   <si>
+    <t xml:space="preserve">www.monitoringresources.org/Document/Method/Details/6859</t>
+  </si>
+  <si>
+    <t xml:space="preserve">www.monitoringresources.org/Document/Method/Details/6875</t>
+  </si>
+  <si>
     <t xml:space="preserve">PoolDp</t>
   </si>
   <si>
+    <t xml:space="preserve">www.monitoringresources.org/Document/Method/Details/6872</t>
+  </si>
+  <si>
     <t xml:space="preserve">wettedWidth_ave</t>
   </si>
   <si>
@@ -1416,9 +1431,6 @@
     <t xml:space="preserve">PctReachInPools</t>
   </si>
   <si>
-    <t xml:space="preserve">www.monitoringresources.org/Document/Method/Details/6844</t>
-  </si>
-  <si>
     <t xml:space="preserve">www.monitoringresources.org/Document/Method/Details/3852</t>
   </si>
   <si>
@@ -1428,30 +1440,27 @@
     <t xml:space="preserve">PctPools</t>
   </si>
   <si>
-    <t xml:space="preserve">www.monitoringresources.org/Document/Method/Details/6859</t>
-  </si>
-  <si>
-    <t xml:space="preserve">www.monitoringresources.org/Document/Method/Details/6875</t>
-  </si>
-  <si>
     <t xml:space="preserve">PoolPct</t>
   </si>
   <si>
-    <t xml:space="preserve">www.monitoringresources.org/Document/Method/Details/6872</t>
-  </si>
-  <si>
     <t xml:space="preserve">www.monitoringresources.org/Document/Method/Details/55</t>
   </si>
   <si>
     <t xml:space="preserve">BNK_AN</t>
   </si>
   <si>
+    <t xml:space="preserve">www.monitoringresources.org/Document/Method/Details/68</t>
+  </si>
+  <si>
     <t xml:space="preserve">BNK_STBLTY</t>
   </si>
   <si>
     <t xml:space="preserve">Stab</t>
   </si>
   <si>
+    <t xml:space="preserve">www.monitoringresources.org/Document/Method/Details/69</t>
+  </si>
+  <si>
     <t xml:space="preserve">www.monitoringresources.org/Document/Method/Details/6797</t>
   </si>
   <si>
@@ -1521,12 +1530,21 @@
     <t xml:space="preserve">XDEPTH_CM</t>
   </si>
   <si>
+    <t xml:space="preserve">www.monitoringresources.org/Document/Method/Details/65</t>
+  </si>
+  <si>
+    <t xml:space="preserve">www.monitoringresources.org/Document/Method/Details/5537</t>
+  </si>
+  <si>
     <t xml:space="preserve">TSS</t>
   </si>
   <si>
     <t xml:space="preserve">Cond</t>
   </si>
   <si>
+    <t xml:space="preserve">www.monitoringresources.org/Document/Method/Details/61</t>
+  </si>
+  <si>
     <t xml:space="preserve">NTL</t>
   </si>
   <si>
@@ -1540,6 +1558,9 @@
   </si>
   <si>
     <t xml:space="preserve">TURB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">www.monitoringresources.org/Document/Method/Details/3806</t>
   </si>
 </sst>
 </file>
@@ -6591,25 +6612,29 @@
       <c r="J39" t="s">
         <v>438</v>
       </c>
-      <c r="K39"/>
+      <c r="K39" t="s">
+        <v>439</v>
+      </c>
       <c r="L39"/>
       <c r="M39" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="N39" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="O39"/>
       <c r="P39"/>
       <c r="Q39" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="R39"/>
       <c r="S39"/>
       <c r="T39" t="s">
-        <v>442</v>
-      </c>
-      <c r="U39"/>
+        <v>443</v>
+      </c>
+      <c r="U39" t="s">
+        <v>433</v>
+      </c>
       <c r="V39"/>
     </row>
     <row r="40">
@@ -6637,12 +6662,12 @@
       </c>
       <c r="I40"/>
       <c r="J40" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="K40"/>
       <c r="L40"/>
       <c r="M40" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="N40"/>
       <c r="O40"/>
@@ -6681,7 +6706,7 @@
         <v>120</v>
       </c>
       <c r="J41" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="K41"/>
       <c r="L41"/>
@@ -6690,12 +6715,12 @@
       <c r="O41"/>
       <c r="P41"/>
       <c r="Q41" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="R41"/>
       <c r="S41"/>
       <c r="T41" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="U41"/>
       <c r="V41"/>
@@ -6732,7 +6757,7 @@
       <c r="K42"/>
       <c r="L42"/>
       <c r="M42" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="N42" t="s">
         <v>146</v>
@@ -6740,7 +6765,7 @@
       <c r="O42"/>
       <c r="P42"/>
       <c r="Q42" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="R42"/>
       <c r="S42"/>
@@ -6775,20 +6800,20 @@
         <v>120</v>
       </c>
       <c r="J43" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="K43"/>
       <c r="L43"/>
       <c r="M43" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="N43" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="O43"/>
       <c r="P43"/>
       <c r="Q43" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="R43"/>
       <c r="S43"/>
@@ -6823,25 +6848,33 @@
         <v>120</v>
       </c>
       <c r="J44" t="s">
-        <v>454</v>
-      </c>
-      <c r="K44"/>
+        <v>455</v>
+      </c>
+      <c r="K44" t="s">
+        <v>456</v>
+      </c>
       <c r="L44"/>
       <c r="M44" t="s">
-        <v>455</v>
+        <v>457</v>
       </c>
       <c r="N44" t="s">
-        <v>456</v>
-      </c>
-      <c r="O44"/>
+        <v>458</v>
+      </c>
+      <c r="O44" t="s">
+        <v>459</v>
+      </c>
       <c r="P44"/>
       <c r="Q44"/>
-      <c r="R44"/>
+      <c r="R44" t="s">
+        <v>460</v>
+      </c>
       <c r="S44"/>
       <c r="T44" t="s">
-        <v>457</v>
-      </c>
-      <c r="U44"/>
+        <v>461</v>
+      </c>
+      <c r="U44" t="s">
+        <v>462</v>
+      </c>
       <c r="V44"/>
     </row>
     <row r="45">
@@ -6871,20 +6904,20 @@
         <v>120</v>
       </c>
       <c r="J45" t="s">
-        <v>458</v>
+        <v>463</v>
       </c>
       <c r="K45"/>
       <c r="L45"/>
       <c r="M45" t="s">
-        <v>459</v>
+        <v>464</v>
       </c>
       <c r="N45" t="s">
-        <v>460</v>
+        <v>465</v>
       </c>
       <c r="O45"/>
       <c r="P45"/>
       <c r="Q45" t="s">
-        <v>461</v>
+        <v>466</v>
       </c>
       <c r="R45"/>
       <c r="S45"/>
@@ -6921,39 +6954,39 @@
         <v>130</v>
       </c>
       <c r="J46" t="s">
-        <v>462</v>
+        <v>467</v>
       </c>
       <c r="K46" t="s">
-        <v>463</v>
+        <v>456</v>
       </c>
       <c r="L46" t="s">
-        <v>464</v>
+        <v>468</v>
       </c>
       <c r="M46" t="s">
-        <v>465</v>
+        <v>469</v>
       </c>
       <c r="N46" t="s">
-        <v>466</v>
+        <v>470</v>
       </c>
       <c r="O46" t="s">
-        <v>467</v>
+        <v>459</v>
       </c>
       <c r="P46"/>
       <c r="Q46"/>
       <c r="R46" t="s">
-        <v>468</v>
+        <v>460</v>
       </c>
       <c r="S46" t="n">
         <v>88</v>
       </c>
       <c r="T46" t="s">
-        <v>469</v>
+        <v>471</v>
       </c>
       <c r="U46" t="s">
-        <v>470</v>
+        <v>462</v>
       </c>
       <c r="V46" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
     </row>
     <row r="47">
@@ -6988,7 +7021,7 @@
       <c r="K47"/>
       <c r="L47"/>
       <c r="M47" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="N47"/>
       <c r="O47"/>
@@ -6999,7 +7032,9 @@
       <c r="T47" t="s">
         <v>164</v>
       </c>
-      <c r="U47"/>
+      <c r="U47" t="s">
+        <v>474</v>
+      </c>
       <c r="V47"/>
     </row>
     <row r="48">
@@ -7034,7 +7069,7 @@
       <c r="K48"/>
       <c r="L48"/>
       <c r="M48" t="s">
-        <v>473</v>
+        <v>475</v>
       </c>
       <c r="N48"/>
       <c r="O48"/>
@@ -7043,9 +7078,11 @@
       <c r="R48"/>
       <c r="S48"/>
       <c r="T48" t="s">
-        <v>474</v>
-      </c>
-      <c r="U48"/>
+        <v>476</v>
+      </c>
+      <c r="U48" t="s">
+        <v>477</v>
+      </c>
       <c r="V48"/>
     </row>
     <row r="49">
@@ -7080,7 +7117,7 @@
         <v>173</v>
       </c>
       <c r="K49" t="s">
-        <v>475</v>
+        <v>478</v>
       </c>
       <c r="L49"/>
       <c r="M49" t="s">
@@ -7090,21 +7127,21 @@
         <v>173</v>
       </c>
       <c r="O49" t="s">
-        <v>476</v>
+        <v>479</v>
       </c>
       <c r="P49"/>
       <c r="Q49" t="s">
-        <v>477</v>
+        <v>480</v>
       </c>
       <c r="R49" t="s">
-        <v>478</v>
+        <v>481</v>
       </c>
       <c r="S49"/>
       <c r="T49" t="s">
         <v>173</v>
       </c>
       <c r="U49" t="s">
-        <v>475</v>
+        <v>478</v>
       </c>
       <c r="V49"/>
     </row>
@@ -7137,34 +7174,34 @@
         <v>130</v>
       </c>
       <c r="J50" t="s">
-        <v>479</v>
+        <v>482</v>
       </c>
       <c r="K50" t="s">
-        <v>475</v>
+        <v>478</v>
       </c>
       <c r="L50"/>
       <c r="M50" t="s">
-        <v>480</v>
+        <v>483</v>
       </c>
       <c r="N50" t="s">
-        <v>481</v>
+        <v>484</v>
       </c>
       <c r="O50" t="s">
-        <v>482</v>
+        <v>485</v>
       </c>
       <c r="P50"/>
       <c r="Q50" t="s">
-        <v>483</v>
+        <v>486</v>
       </c>
       <c r="R50" t="s">
-        <v>478</v>
+        <v>481</v>
       </c>
       <c r="S50"/>
       <c r="T50" t="s">
-        <v>484</v>
+        <v>487</v>
       </c>
       <c r="U50" t="s">
-        <v>475</v>
+        <v>478</v>
       </c>
       <c r="V50"/>
     </row>
@@ -7197,32 +7234,32 @@
         <v>130</v>
       </c>
       <c r="J51" t="s">
-        <v>485</v>
+        <v>488</v>
       </c>
       <c r="K51" t="s">
-        <v>475</v>
+        <v>478</v>
       </c>
       <c r="L51"/>
       <c r="M51" t="s">
-        <v>486</v>
+        <v>489</v>
       </c>
       <c r="N51" t="s">
-        <v>487</v>
+        <v>490</v>
       </c>
       <c r="O51" t="s">
-        <v>476</v>
+        <v>479</v>
       </c>
       <c r="P51"/>
       <c r="Q51"/>
       <c r="R51" t="s">
-        <v>478</v>
+        <v>481</v>
       </c>
       <c r="S51"/>
       <c r="T51" t="s">
-        <v>488</v>
+        <v>491</v>
       </c>
       <c r="U51" t="s">
-        <v>475</v>
+        <v>478</v>
       </c>
       <c r="V51"/>
     </row>
@@ -7256,7 +7293,7 @@
       </c>
       <c r="J52"/>
       <c r="K52" t="s">
-        <v>475</v>
+        <v>478</v>
       </c>
       <c r="L52"/>
       <c r="M52" t="s">
@@ -7264,16 +7301,20 @@
       </c>
       <c r="N52"/>
       <c r="O52" t="s">
-        <v>489</v>
+        <v>492</v>
       </c>
       <c r="P52"/>
       <c r="Q52"/>
-      <c r="R52"/>
+      <c r="R52" t="s">
+        <v>481</v>
+      </c>
       <c r="S52"/>
       <c r="T52" t="s">
         <v>185</v>
       </c>
-      <c r="U52"/>
+      <c r="U52" t="s">
+        <v>478</v>
+      </c>
       <c r="V52"/>
     </row>
     <row r="53">
@@ -7306,7 +7347,7 @@
       </c>
       <c r="J53"/>
       <c r="K53" t="s">
-        <v>475</v>
+        <v>478</v>
       </c>
       <c r="L53"/>
       <c r="M53" t="s">
@@ -7314,16 +7355,20 @@
       </c>
       <c r="N53"/>
       <c r="O53" t="s">
-        <v>489</v>
+        <v>492</v>
       </c>
       <c r="P53"/>
       <c r="Q53"/>
-      <c r="R53"/>
+      <c r="R53" t="s">
+        <v>481</v>
+      </c>
       <c r="S53"/>
       <c r="T53" t="s">
         <v>188</v>
       </c>
-      <c r="U53"/>
+      <c r="U53" t="s">
+        <v>478</v>
+      </c>
       <c r="V53"/>
     </row>
     <row r="54">
@@ -7355,20 +7400,20 @@
         <v>130</v>
       </c>
       <c r="J54" t="s">
-        <v>490</v>
+        <v>493</v>
       </c>
       <c r="K54" t="s">
-        <v>475</v>
+        <v>478</v>
       </c>
       <c r="L54"/>
       <c r="M54"/>
       <c r="N54"/>
       <c r="O54" t="s">
-        <v>489</v>
+        <v>492</v>
       </c>
       <c r="P54"/>
       <c r="Q54" t="s">
-        <v>491</v>
+        <v>494</v>
       </c>
       <c r="R54"/>
       <c r="S54"/>
@@ -7405,28 +7450,28 @@
         <v>130</v>
       </c>
       <c r="J55" t="s">
-        <v>492</v>
+        <v>495</v>
       </c>
       <c r="K55" t="s">
-        <v>493</v>
+        <v>496</v>
       </c>
       <c r="L55"/>
       <c r="M55" t="s">
-        <v>494</v>
+        <v>497</v>
       </c>
       <c r="N55"/>
       <c r="O55" t="s">
-        <v>482</v>
+        <v>485</v>
       </c>
       <c r="P55"/>
       <c r="Q55"/>
       <c r="R55"/>
       <c r="S55"/>
       <c r="T55" t="s">
-        <v>484</v>
+        <v>487</v>
       </c>
       <c r="U55" t="s">
-        <v>482</v>
+        <v>485</v>
       </c>
       <c r="V55"/>
     </row>
@@ -7462,21 +7507,21 @@
       <c r="K56"/>
       <c r="L56"/>
       <c r="M56" t="s">
-        <v>495</v>
+        <v>498</v>
       </c>
       <c r="N56"/>
       <c r="O56" t="s">
-        <v>482</v>
+        <v>485</v>
       </c>
       <c r="P56"/>
       <c r="Q56"/>
       <c r="R56"/>
       <c r="S56"/>
       <c r="T56" t="s">
-        <v>488</v>
+        <v>491</v>
       </c>
       <c r="U56" t="s">
-        <v>482</v>
+        <v>485</v>
       </c>
       <c r="V56"/>
     </row>
@@ -7830,13 +7875,13 @@
       <c r="K65"/>
       <c r="L65"/>
       <c r="M65" t="s">
-        <v>496</v>
+        <v>499</v>
       </c>
       <c r="N65"/>
       <c r="O65"/>
       <c r="P65"/>
       <c r="Q65" t="s">
-        <v>497</v>
+        <v>500</v>
       </c>
       <c r="R65"/>
       <c r="S65"/>
@@ -7917,7 +7962,9 @@
       <c r="R67"/>
       <c r="S67"/>
       <c r="T67"/>
-      <c r="U67"/>
+      <c r="U67" t="s">
+        <v>501</v>
+      </c>
       <c r="V67"/>
     </row>
     <row r="68">
@@ -8901,21 +8948,25 @@
         <v>314</v>
       </c>
       <c r="J93"/>
-      <c r="K93"/>
+      <c r="K93" t="s">
+        <v>502</v>
+      </c>
       <c r="L93"/>
       <c r="M93"/>
       <c r="N93"/>
       <c r="O93"/>
       <c r="P93"/>
       <c r="Q93" t="s">
-        <v>498</v>
+        <v>503</v>
       </c>
       <c r="R93"/>
       <c r="S93"/>
       <c r="T93" t="s">
-        <v>499</v>
-      </c>
-      <c r="U93"/>
+        <v>504</v>
+      </c>
+      <c r="U93" t="s">
+        <v>505</v>
+      </c>
       <c r="V93"/>
     </row>
     <row r="94">
@@ -8954,7 +9005,7 @@
       <c r="O94"/>
       <c r="P94"/>
       <c r="Q94" t="s">
-        <v>500</v>
+        <v>506</v>
       </c>
       <c r="R94"/>
       <c r="S94"/>
@@ -8998,7 +9049,7 @@
       <c r="O95"/>
       <c r="P95"/>
       <c r="Q95" t="s">
-        <v>501</v>
+        <v>507</v>
       </c>
       <c r="R95"/>
       <c r="S95"/>
@@ -9044,7 +9095,7 @@
       <c r="O96"/>
       <c r="P96"/>
       <c r="Q96" t="s">
-        <v>502</v>
+        <v>508</v>
       </c>
       <c r="R96"/>
       <c r="S96"/>
@@ -9093,7 +9144,9 @@
       <c r="R97"/>
       <c r="S97"/>
       <c r="T97"/>
-      <c r="U97"/>
+      <c r="U97" t="s">
+        <v>505</v>
+      </c>
       <c r="V97"/>
     </row>
     <row r="98">
@@ -9126,13 +9179,13 @@
       <c r="K98"/>
       <c r="L98"/>
       <c r="M98" t="s">
-        <v>503</v>
+        <v>509</v>
       </c>
       <c r="N98"/>
       <c r="O98"/>
       <c r="P98"/>
       <c r="Q98" t="s">
-        <v>504</v>
+        <v>510</v>
       </c>
       <c r="R98"/>
       <c r="S98"/>
@@ -9167,7 +9220,9 @@
         <v>338</v>
       </c>
       <c r="J99"/>
-      <c r="K99"/>
+      <c r="K99" t="s">
+        <v>511</v>
+      </c>
       <c r="L99"/>
       <c r="M99"/>
       <c r="N99"/>

</xml_diff>